<commit_message>
14:15 time 21.10.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -1052,6 +1052,1897 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Avdusamatova Maftuna Davronjon qizi</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>AB1660675</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>612</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Uchkoʻprik tumani</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>998911504540</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Bekchanova Dilnoza Yusupboy qizi</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>AB7327834</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>613</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Shovot tumani</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>998914225303</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Ollamova Latofat Yusupbayevna</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>AB2074711</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>614</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Yangibozor tumani</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>998978566764</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Rajabova Gulrux Qudratovna</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>AD7589225</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>615</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Yangibozor tumani</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>998973639296</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Usmonova Maftunaxon Dilshodjon qizi</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>AD3251163</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>616</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Uchkoʻprik tumani</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>998991080401</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Sirojiddinova Mavluda</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>AA8409833</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>617</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>998938487005</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Sirojiddinova Mavludaxon</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>AB8409833</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>618</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>998938487005</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Nuraddinova Zuxra Shuxrat qizi</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>AD3782647</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>619</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>998975283282</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>09-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Mamasoliyeva E'tibor Akbarovna</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>AD4957782</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>620</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Pastdargʻom tumani</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>998915393522</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>10-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Axmadjonova Gulshidaxon Xidoyatjon qizi</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>AA9217449</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>621</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Fargʻona tumani</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>998911181500</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Sultanova Gulmira Togizbaevna</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>AD5310078</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>622</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Qoraoʻzak tumani</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>998937162185</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Abdubannobova Xumorabonu Muzaffar qizi</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>AD4736522</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>623</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Toshloq tumani</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>+998916578683</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Iskandarova Aydana Ibadullaevna</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>AD3148861</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>624</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Konimex tumani</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>+99833600094</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Isayeva Diana Abduraim qizi</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>AD7768158</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>625</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Yangiyoʻl tumani</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>998946662706</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Xabibullayeva Manzura
+Fayzullayevna</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>AD8003136</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>626</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Gʻallaorol tumani</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>998935496866</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Xo'janova Dildora Gulomjon qizi</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>AB0110701</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>626</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Yangihayot tumani</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>998977668493</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Abdusamatova Shaxnoza Gulomjon qizi</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>AD4439645</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>627</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Buloqboshi tumani</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>998999055570</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Tursunaliyeva Karimaxon Shuhratjon qizi</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>AD4447848</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>628</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Pop tumani</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>998935374993</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>12-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Murtazoyeva Sitora Akmal qizi</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>AB7859105</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>629</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Gʻijduvon tumani</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>998912406349</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>12-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Tairova Zarnigor Ibragim qizi</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>AC2686542</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>630</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Boʻka tumani</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>998951670686</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>12-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Mamatmurodova Sayyora Anorqul qizi</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>AD8874981</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>631</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Zomin tumani</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>998946488492</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>12-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Suyarov Tolibjon Melikuzievich</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>AA8527028</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>632</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Uchkoʻprik tumani</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>998972061000</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>13-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>To'lqinova Mahliyo Murodjon qizi</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>AB8526847</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>633</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Piskent tumani</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>998953500128</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>14-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Karimova Zulfiyaxon Xudoberdi qizi</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>AD0747249</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>634</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Quva tumani</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>998943922323</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>14-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Sobirova Ozoda</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>AC1708058</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>635</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Zomin tumani</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>998971261595</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>14-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Rashidova Dilfuza Nasimovna</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>AB4997664</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>636</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Navoiy shahri</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>998913396565</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>14-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Xabibullayeva Manzura Fayzullayevna</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>AD8003136</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>637</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Gʻallaorol tumani</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>998935496866</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>14-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Tangirberdiyeva Gulnoza</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>AD3934104</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>638</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Bulungʻur tumani</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>+998990943526</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>14-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Umarova Barnoxon Madaminbekovna</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>AD5896366</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>639</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>998993281001</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>15-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Qudratova Dilfuza</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>AA9690488</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>640</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Nishon tumani</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>998994070485</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>15-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Maxmudjonova Go'zal G'iyosiddin qizi</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>AB7092108</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>641</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>998931921141</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>15-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Aliboyeva Nazira Aliboy qizi</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>AD1070599</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>642</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Chiroqchi tumani</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>998919478334</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>17-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Abduraxmonova Xilola Sultonboyevna</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>AD3102536</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>643</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Mingbuloq tumani</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>998999338585</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>17-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>AVG'ONOVA SARVINOZ BAXTIYOR QIZI</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>AB5543647</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>644</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Boysun tumani</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>998900767298</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>17-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Sultonova Dilnoza Xudoykulovna</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>AD8341857</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>645</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Sirdaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Boyovut tumani</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>+998993234687</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>17-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Doliyeva Kamola Normo'min qizi</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>AD4810777</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>646</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>998882839397</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>17-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Abdumajitova Laylo Abdumurod qizi</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>AC0451245</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>647</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Piskent tumani</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>998931686880</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>17-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Orinboyeva NIGORAHON SHAMSIDINOVNA</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>AD3684327</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>648</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Xoʻjaobod tumani</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>998905293342</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>18-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Rabbimova Marjona Vohobiddin qizi</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>AD4725837</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>649</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>998934621333</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>18-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Po'latova Shaxzoda bekmirza qizi</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>AD3798796</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Kosonsoy tumani</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>998907540390</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>18-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Rasulova Lobar Tulqinjon qizi</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>AC2563440</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>651</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>998940892950</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>19-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Nurmurotova Gullola Baxodir qizi</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>AB3134499</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>652</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>998996726108</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>19-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>O'razimbetova Nilufar Sadullayevna</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>KA0744767</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>653</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Amudaryo tumani</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>998949092924</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>19-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Muxtorova Iqboloy Akmal qizi</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>AA9276244</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>654</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Qiziltepa tumani</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>998900874656</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>21-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Sharopova Madina G'ayrat qizi</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>AD4529888</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>655</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Gʻijduvon tumani</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>998912441105</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>21-10-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
12:16 time 22.10.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -2943,6 +2943,132 @@
         </is>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Normurodova Fotima Asaddin qizi</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>AD3672634</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>656</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Paxtachi tumani</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>998934112173</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>21-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Husainova Laylo Allayorovna</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>AD4912996</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>657</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Peshku tumani</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>998907158671</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>21-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Mamatova Nigora Yo'ldosh qizi</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>AC0870202</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>658</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Sherobod tumani</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>998937092606</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>22-10-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
21:11 time 24.10.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -3069,6 +3069,426 @@
         </is>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Suyarova Oygul Alijonovna</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>AD2406777</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>659</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Uchkoʻprik tumani</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>998886288668</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>22-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Doniyorova Rushana</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>AA8597474</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>660</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Ishtixon tumani</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>998999477280</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>22-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Oteshova Nilufar Muxtor qizi</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>AA8915214</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>661</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Chinoz tumani</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>998889480203</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Fozilova Shalola Ashurali qizi</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>AA9160420</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>662</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Bagʻdod tumani</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>998995151300</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Salomova Nafosat Amriddinovna</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>AD8677620</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>663</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Gʻijduvon tumani</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>998937947800</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Qoraboyeva Umida Usmonaliyevna</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>AD3440246</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>664</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Kosonsoy tumani</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>998941517977</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Sobirova Muxlisaxon Inomjon qizi</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>AC2423096</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>665</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Quva tumani</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>998907814346</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Holturayeva Mohigul Omonovna</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>AB1849370</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>666</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Termiz tumani</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>998919083078</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Nurmurotova Gullola Bahodir qizi</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>AB3134499</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>667</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>998996726108</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>23-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Mexmanova Munisa Musaxanovna</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>AD7063844</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>668</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Chortoq tumani</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>998941735001</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>24-10-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
16:46 time 30.10.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -3489,6 +3489,636 @@
         </is>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Rasulova Odina Abduvaliyevna</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Amaliy psixologiya 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>AD3305485</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>669</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Rishton tumani</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>998905633728</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>25-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Alimova Hayotxon Qobiljonovna</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>AD5159476</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>670</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Jalaquduq tuman</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>998916126213</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>25-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Madg'oziyeva Sabohat Xatamovna</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>AD3227666</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>671</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Toshloq tumani</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>998916580488</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>25-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Omonkeldiyeva Nilufar Shuxrat qizi</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>AD1581888</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>672</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>998915227679</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>25-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Xaydarova Dilfuza Ikromjon qizi</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>AD0898964</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>673</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Oltiariq tumani</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>998916642168</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>26-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Subhonova Farida Islomiddin qizi</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Amaliy psixologiya 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>AB4455226</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>674</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Pastdargʻom tumani</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>998946838894</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>26-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Sadullayeva Nodira Saparbay qizi</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>AB9081455</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>675</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Yangibozor tumani</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>998943296838</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>26-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Elboyeva Nazokat Otabek qizi</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>AB7009475</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>676</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Karmana tumani</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>998935614006</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>28-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Yuldosheva Oybibi Selxanovna</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>AB9839541</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>677</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>998993808528</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>28-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Xolillayeva Kumushoy Ikromjon qizi</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>AD4560577</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>678</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Amudaryo tumani</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>998971705770</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>28-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Normamatov Hamrozbek Xusniddin o'g'li</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>AC0380497</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>679</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Kattaqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>998936066607</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>29-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Kiyasova Ulmeken Ilyas qizi</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>KA0680487</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>680</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Qoʻngʻirot tumani</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>998994554845</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>29-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Axunova Shohzodaxon Olim qizi</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>AD1635577</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>681</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>998998009889</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>30-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Haydarova Maftuna Haliljon qizi</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>AD6997411</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>682</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Oltiariq tumani</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>998931690141</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>30-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Muhtorova Nargiza Abduvositovna</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>AD5529844</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>683</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>998999013032</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>30-10-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
11:26 time 01.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -4119,6 +4119,342 @@
         </is>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Aliyeva Mahliyo Murodjon qizi</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>AD8955000</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>684</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Piskent tumani</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>998953500128</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Saxtabova Umidaxon Bekxo'ja qizi</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>AD6680957</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>685</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Yangiyoʻl tumani</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>998930486446</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Qipchakova Etiborxon Yuldashevna</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>AD8410114</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>686</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>998911440526</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Djaborova Marhaboxon Zokirjonovna</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>AD1322435</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>687</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Ohangaron tumani</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>+998931893234</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Axtamova Marjona Utkir qizi</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>AC0716066</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>688</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Navbahor tumani</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>998505064800</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Zokirova Soliha Abduraxim qizi</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>AD0626175</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>689</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Shayxontohur tumani</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>998974335353</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>31-10-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Yo'ldosheva Mohlaroyim To'ymurod qizi</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>AD0130593</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>690</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Qiziltepa tumani</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>998999264272</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Rahmonova Muxlisa Gofurgon qizi</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>AB2555334</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>691</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Narpay tumani</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>998978927477</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
17:54 time 04.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
@@ -4455,6 +4455,552 @@
         </is>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Abdullaeva Xilola Ilhomovna</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>AB0449918</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>692</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Xiva tumani</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>998990610110</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>01-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Qurbonova Mohigul Esonali qizi</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>AD4463924</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>693</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Beshariq tumani</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>998948263202</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Djabborova Rushana Odil qizi</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>AB5761267</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>694</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Gʻijduvon tumani</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>998916490504</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Sharibova Madina Farxodjon qizi</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>AD4491495</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>695</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Qoʻrgʻontepa tumani</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>998996909708</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Nazirbayeva Dildora Xamza qizi</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>AD3665614</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>696</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Gurlan tumani</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>998972021510</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Kenjayeva Firuzabonu Avazbek qizi</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>AC1274290</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>697</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Izboskan tuman</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>998337200907</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Qayumova Xolidaxon Shuxratovna</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>AD5502952</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>698</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>998900555522</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>02-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Kamolova Rushana Jamilovna</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>AD4512393</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>699</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Ohangaron tumani</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>998909481022</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>03-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Xudayberdiyeva Fotima Oybek qizi</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>AB6207982</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>700</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Nishon tumani</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>998908747305</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>03-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Hamidova Muxtabar Obidovna</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>AB2567833</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>701</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Tomdi tumani</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>998936631068</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>03-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Kurbonova Feruza Baxtiyor qizi</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>AA9126315</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>702</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Kattaqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>998939958881</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>04-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Ismoilova Nozima Alisherovna</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>AD2465041</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>703</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>998909343336</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>04-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Umarova Qumriyahon Qurbonovna</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>AD8990709</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>704</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Konimex tumani</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>998934311981</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>04-11-2024</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
8:57 time 22.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I147"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
       <selection activeCell="A147" sqref="A147:XFD147"/>
@@ -6650,6 +6650,1082 @@
         </is>
       </c>
     </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Rahmonova Oysuluv Mehmonaliyevna</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>AB5022316</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>744</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Baliqchi tumani</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>998956767474</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>14-11-2024</t>
+        </is>
+      </c>
+      <c r="I148" t="inlineStr">
+        <is>
+          <t>+998957677474</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Sobirova Ismigul Bahromjon qizi</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>AD2393298</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>745</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>998912032308</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>14-11-2024</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>+998912032308</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Muminova Mavludaxon Mahmudovna</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>AC2511867</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>746</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>998905407059</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>15-11-2024</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>+998905407059</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Ahmedova Nilufar Mirzaazizovna</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>AA7377260</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>747</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Shahrixon tuman</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>998500721276</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>18-11-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>Samiyeva Farida Xudoyberdi qizi</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>AD7058036</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>748</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Arnasoy tumani</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>998936072294</t>
+        </is>
+      </c>
+      <c r="H152" t="inlineStr">
+        <is>
+          <t>18-11-2024</t>
+        </is>
+      </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>+998936072294</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Sobirova Zarnigor Sobirovna</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>AD3746455</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>749</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Qarshi tumani</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>998500072344</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>18-11-2024</t>
+        </is>
+      </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>+998905180033</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>Otaqoziyeva Gulhayo Mahmudjon qizi</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>AD1672467</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>750</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>998910596680</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>+998910596680</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Rasilova Sevinch Ilhomboyevna</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>AD6148106</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>751</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Yangihayot tumani</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>998770723424</t>
+        </is>
+      </c>
+      <c r="H155" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>+998770273424</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Norqulova Muqaddas Abdumannon qizi</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>AD9376541</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>752</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Shahrixon tuman</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>998902201013</t>
+        </is>
+      </c>
+      <c r="H156" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I156" t="inlineStr">
+        <is>
+          <t>+998902201013</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>TO'XSANOVA FERUZA SOBIROVNA</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>AD7550400</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>753</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Qiziltepa tumani</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>998912508529</t>
+        </is>
+      </c>
+      <c r="H157" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I157" t="inlineStr">
+        <is>
+          <t>+998912508529</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>TO'XSANOVA FERUZA SOBIROVNA</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>AD7550400</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>753</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Qiziltepa tumani</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>998912508529</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>+998912508529</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>Quvondiqova Huriyat Bahronovna</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>AD2409734</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>753</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Mirobod tumani</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>+998950038686</t>
+        </is>
+      </c>
+      <c r="H159" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I159" t="inlineStr">
+        <is>
+          <t>+998950038686</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Hasanova Sevara ABDURAIMOVNA</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>AA9027122</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>753</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Uzun tumani</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>998916158686</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>+998904108161</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Sadriddinova Shahribonu Qoldosh qizi</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>AB0664921</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>754</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Nurota tumani</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>998941471804</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>+998942542111</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Quvondiqova Huriyat Bahronovna</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>AD2409734</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>755</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Mirobod tumani</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>+998950038686</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>+998950038686</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>TO'XSANOVA FERUZA SOBIROVNA</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>AD7550400</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>756</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Qiziltepa tumani</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>998912508529</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>19-11-2024</t>
+        </is>
+      </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>+998912508529</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Saparbayeva Xurshidaxon Dostonbek qizi</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>AD0018405</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>757</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>998905284303</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>20-11-2024</t>
+        </is>
+      </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>+998905284303</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Choriyeva Dilafruz Shuhrat qizi</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>AD6113797</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>758</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Qarshi tumani</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>998935400332</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>21-11-2024</t>
+        </is>
+      </c>
+      <c r="I165" t="inlineStr">
+        <is>
+          <t>+998507200332</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>Shukurlayeva Sabohat Nurlayevna</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>AD7962143</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>759</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Gurlan tumani</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>998993486603</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>21-11-2024</t>
+        </is>
+      </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>+998993486603</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Yuldasheva Irodaxon Raimqul qizi</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Amaliy psixologiya 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>AC2714983</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>760</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Yakkabogʻ tumani</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>998973095203</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>21-11-2024</t>
+        </is>
+      </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>+998973095203</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Sotvoldiyeva Nozima Qodirjonovna</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>AD4032668</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>761</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Bagʻdod tumani</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>998917373670</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>21-11-2024</t>
+        </is>
+      </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>+998917373670</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Buranova Shaxnoza Olimovna</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>AD3858103</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>762</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Sharof Rashidov tumani</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>998902977667</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>21-11-2024</t>
+        </is>
+      </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>+998940687667</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Safarova Madina  Baxtiyor qizi</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>AB8322263</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>763</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Denov tumani</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>998975342848</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>21-11-2024</t>
+        </is>
+      </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>+998975342847</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
11:45 time 22.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I170"/>
+  <dimension ref="A1:I171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
       <selection activeCell="A147" sqref="A147:XFD147"/>
@@ -7726,6 +7726,53 @@
         </is>
       </c>
     </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Amirov Akrom</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>AA7879988</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>764</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Tomdi tumani</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>+12676860109</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>22-11-2024</t>
+        </is>
+      </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
11:51 time 26.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I176"/>
+  <dimension ref="A1:I180"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
       <selection activeCell="A171" sqref="A171:XFD171"/>
@@ -8008,6 +8008,194 @@
         </is>
       </c>
     </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Hamroyeva Nigora Husan Qizi</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>AD3548929</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>770</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>998934319253</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>23-11-2024</t>
+        </is>
+      </c>
+      <c r="I177" t="inlineStr">
+        <is>
+          <t>+998934319253</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Saxibova Muxayyo Saidjonovna</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>AD7351130</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>771</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Qibray tumani</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>998998313914</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>23-11-2024</t>
+        </is>
+      </c>
+      <c r="I178" t="inlineStr">
+        <is>
+          <t>+998505003914</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Mahmudova Dilnoza Xolboy qizi</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>AB7598097</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>772</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Gʻallaorol tumani</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>998941603726</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>26-11-2024</t>
+        </is>
+      </c>
+      <c r="I179" t="inlineStr">
+        <is>
+          <t>+998941603726</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Usarova Tursunoy Umarovna</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>AA9143291</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>773</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Sharof Rashidov tumani</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>998503014091</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>26-11-2024</t>
+        </is>
+      </c>
+      <c r="I180" t="inlineStr">
+        <is>
+          <t>+998503014091</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
11:21 time 28.11.2024 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I180"/>
+  <dimension ref="A1:I184"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
       <selection activeCell="A171" sqref="A171:XFD171"/>
@@ -8196,6 +8196,194 @@
         </is>
       </c>
     </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Asqarova Zarnigor Asqarovna</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>AA8561113</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>774</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Denov tumani</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>998900711166</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>27-11-2024</t>
+        </is>
+      </c>
+      <c r="I181" t="inlineStr">
+        <is>
+          <t>+998900711166</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Shermetova Intizor Hasan qizi</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>AB5889957</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>775</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Shovot tumani</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>998913809033</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>27-11-2024</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>+998913809033</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Abdullayeva Oltinoy Choriyevna</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>AB3378808</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>776</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Uzun tumani</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>998948626560</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>27-11-2024</t>
+        </is>
+      </c>
+      <c r="I183" t="inlineStr">
+        <is>
+          <t>+998948626560</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Yuldashov Jaloliddin Sharofiddin o'g'li</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>AB0767338</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>777</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Hazorasp tumani</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>998973633103</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>28-11-2024</t>
+        </is>
+      </c>
+      <c r="I184" t="inlineStr">
+        <is>
+          <t>+998973633103</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
17:11 time 03.01.2025 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I184"/>
+  <dimension ref="A1:I274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
       <selection activeCell="A171" sqref="A171:XFD171"/>
@@ -8384,6 +8384,4225 @@
         </is>
       </c>
     </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Soqiyeva Gulxumor Umidjon qizi</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>AB6127104</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>778</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Andijon tuman</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>998500755457</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>30-11-2024</t>
+        </is>
+      </c>
+      <c r="I185" t="inlineStr">
+        <is>
+          <t>+998500755457</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Qodirova Gulshoda To'lqin qizi</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>AD5260977</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>779</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Ishtixon tumani</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>998972441298</t>
+        </is>
+      </c>
+      <c r="H186" t="inlineStr">
+        <is>
+          <t>01-12-2024</t>
+        </is>
+      </c>
+      <c r="I186" t="inlineStr">
+        <is>
+          <t>+998972441298</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Abdullaeva Marifat Kamiljanovna</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>KA1204694</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>780</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Amudaryo tumani</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>998937173458</t>
+        </is>
+      </c>
+      <c r="H187" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+      <c r="I187" t="inlineStr">
+        <is>
+          <t>+998937173458</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Nurxonova Sadoqat Ismoilovna</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>AB1046108</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>781</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Qumqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>998994215338</t>
+        </is>
+      </c>
+      <c r="H188" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+      <c r="I188" t="inlineStr">
+        <is>
+          <t>+998994215338</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Sanoyeva Shaxnoza Temirovna</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>AA9881075</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>782</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Qiziltepa tumani</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>998906180151</t>
+        </is>
+      </c>
+      <c r="H189" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+      <c r="I189" t="inlineStr">
+        <is>
+          <t>+998992898330</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Abdukarimova Mavluda Muxtorjon qizi</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>AB9956355</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>783</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Chust tumani</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>998903489848</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+      <c r="I190" t="inlineStr">
+        <is>
+          <t>+998903489848</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Bazarova Dilbar Buriyevna</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>AD3614694</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>784</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Doʻstlik tumani</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>998992381018</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>+998992381018</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>AD5700831</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>785</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Sergeli tumani</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>998992030999</t>
+        </is>
+      </c>
+      <c r="H192" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Xolmirzoyeva Madina Akbaraliyevna</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>AD3634729</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>786</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Bekobod tumani</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>998908228786</t>
+        </is>
+      </c>
+      <c r="H193" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+      <c r="I193" t="inlineStr">
+        <is>
+          <t>+998908228786</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>Nizomova Gulzoda Aktamovna</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>AD5021881</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>787</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Kattaqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>998995979408</t>
+        </is>
+      </c>
+      <c r="H194" t="inlineStr">
+        <is>
+          <t>02-12-2024</t>
+        </is>
+      </c>
+      <c r="I194" t="inlineStr">
+        <is>
+          <t>+998995979408</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Baxodirova Umida Ixtiyor qizi</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>AB3367797</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>788</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Shovot tumani</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>998956761612</t>
+        </is>
+      </c>
+      <c r="H195" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I195" t="inlineStr">
+        <is>
+          <t>+998956761612</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Nizomova Gulzoda Aktamovna</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>AD5021881</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>789</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Kattaqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>998995979408</t>
+        </is>
+      </c>
+      <c r="H196" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I196" t="inlineStr">
+        <is>
+          <t>+998995979408</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Bekbayeva Rayhon</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>AB1751175</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>790</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>998991643609</t>
+        </is>
+      </c>
+      <c r="H197" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA
+YULDUZ 
+RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>791</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Bekbayeva Rayhon Rashidovna</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>AB1751175</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>790</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>998991643609</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I199" t="inlineStr">
+        <is>
+          <t>+998991643609</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Jo'rayeva Dilnoza Zafarjon qizi</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>AC2916394</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>791</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>998884152445</t>
+        </is>
+      </c>
+      <c r="H200" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I200" t="inlineStr">
+        <is>
+          <t>+998906328005</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Mirzakarimova Hilola Erkinovna</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>AD2445234</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>792</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>Bekobod tumani</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>998931266027</t>
+        </is>
+      </c>
+      <c r="H201" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I201" t="inlineStr">
+        <is>
+          <t>+998931266027</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA
+YULDUZ 
+RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>793</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H202" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I202" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Yakubova Nilufar Shavkatovna</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>AB4268371</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>793</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>Qoʻshkoʻpir tumani</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>998991438755</t>
+        </is>
+      </c>
+      <c r="H203" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I203" t="inlineStr">
+        <is>
+          <t>+998881438755</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Xolmatova Xonzodaxon Sobirjonovna</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>Amaliy psixologiya 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>AA7710468</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>794</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Buloqboshi tumani</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>998914937007</t>
+        </is>
+      </c>
+      <c r="H204" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I204" t="inlineStr">
+        <is>
+          <t>+998914937007</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA
+YULDUZ 
+RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>795</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H205" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I205" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Xolmatova Xonzodaxon Sobirjonovna</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>Amaliy psixologiya 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>AA7710468</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>795</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Buloqboshi tumani</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>998914937007</t>
+        </is>
+      </c>
+      <c r="H206" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I206" t="inlineStr">
+        <is>
+          <t>+998914937007</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA
+YULDUZ 
+RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>796</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H207" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I207" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Sharipova Sadoqat Azamatovna</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>AB0019928</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>796</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Qiziltepa tumani</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>998914388701</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Muratova Shaxnoza Uktamovna</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>AD5700831</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>797</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Sergeli tumani</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>998992030999</t>
+        </is>
+      </c>
+      <c r="H209" t="inlineStr">
+        <is>
+          <t>03-12-2024</t>
+        </is>
+      </c>
+      <c r="I209" t="inlineStr">
+        <is>
+          <t>+998992030999</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Ibotova Yulduz Farxod qizi</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>AD0513626</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>798</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>998942201996</t>
+        </is>
+      </c>
+      <c r="H210" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+      <c r="I210" t="inlineStr">
+        <is>
+          <t>+998942201996</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA
+YULDUZ 
+RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>799</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H211" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+      <c r="I211" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Qudratova Sanobar Boysariyevna</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>AD7352629</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>799</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>Qamashi tumani</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>998992668109</t>
+        </is>
+      </c>
+      <c r="H212" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+      <c r="I212" t="inlineStr">
+        <is>
+          <t>+998992668109</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA
+YULDUZ 
+RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H213" t="inlineStr">
+        <is>
+          <t>04-12-2024</t>
+        </is>
+      </c>
+      <c r="I213" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Matkarimova Aysha Shavkatovna</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>KA1249468</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Toʻrtkoʻl tumani</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>998977878881</t>
+        </is>
+      </c>
+      <c r="H214" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I214" t="inlineStr">
+        <is>
+          <t>+998977878881</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Karimova Dilfuza Rustam qizi</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>AD0782778</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>801</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>998935630603</t>
+        </is>
+      </c>
+      <c r="H215" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I215" t="inlineStr">
+        <is>
+          <t>+998935630603</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA
+YULDUZ 
+RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>802</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H216" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I216" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>RAYMBAYEVA YULDUZ RAMANBERGANOVNA</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>AD9192789</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>802</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>Beruniy tumani</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>998913828305</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I217" t="inlineStr">
+        <is>
+          <t>+998913828305</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Nafasova Feruza Baxriddin qizi</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>AB7037616</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>803</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>998990021743</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>+998901277789</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Nomonova Gulhayo Shuhratjon qizi</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>AC2702207</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>804</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F219" t="inlineStr">
+        <is>
+          <t>Rishton tumani</t>
+        </is>
+      </c>
+      <c r="G219" t="inlineStr">
+        <is>
+          <t>998913266096</t>
+        </is>
+      </c>
+      <c r="H219" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I219" t="inlineStr">
+        <is>
+          <t>+998913266096</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Muhammedova Mohitobon</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>AB5781434</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>805</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F220" t="inlineStr">
+        <is>
+          <t>Toshloq tumani</t>
+        </is>
+      </c>
+      <c r="G220" t="inlineStr">
+        <is>
+          <t>998911228833</t>
+        </is>
+      </c>
+      <c r="H220" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I220" t="inlineStr">
+        <is>
+          <t>+998911228833</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Jumayev Sirojiddin Poyanovich</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>AC0665134</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>806</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F221" t="inlineStr">
+        <is>
+          <t>Qamashi tumani</t>
+        </is>
+      </c>
+      <c r="G221" t="inlineStr">
+        <is>
+          <t>998904254353</t>
+        </is>
+      </c>
+      <c r="H221" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I221" t="inlineStr">
+        <is>
+          <t>+998999654353</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Saidova Sitora Nishon qizi</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>AD7582892</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>807</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F222" t="inlineStr">
+        <is>
+          <t>Sergeli tumani</t>
+        </is>
+      </c>
+      <c r="G222" t="inlineStr">
+        <is>
+          <t>998936626039</t>
+        </is>
+      </c>
+      <c r="H222" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I222" t="inlineStr">
+        <is>
+          <t>+998936626039</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Xolmatova Xonzodaxon Sobirjonovna</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>Amaliy psixologiya 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>AD9681960</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>807</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F223" t="inlineStr">
+        <is>
+          <t>Buloqboshi tumani</t>
+        </is>
+      </c>
+      <c r="G223" t="inlineStr">
+        <is>
+          <t>998914937007</t>
+        </is>
+      </c>
+      <c r="H223" t="inlineStr">
+        <is>
+          <t>05-12-2024</t>
+        </is>
+      </c>
+      <c r="I223" t="inlineStr">
+        <is>
+          <t>+998914937007</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Narzullayeva Moxibonu Sharofiddin qizi</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>AC2854785</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>808</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F224" t="inlineStr">
+        <is>
+          <t>Uzun tumani</t>
+        </is>
+      </c>
+      <c r="G224" t="inlineStr">
+        <is>
+          <t>998909750350</t>
+        </is>
+      </c>
+      <c r="H224" t="inlineStr">
+        <is>
+          <t>06-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Sariqova Dilorom Namozovna</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>AB0423950</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>809</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F225" t="inlineStr">
+        <is>
+          <t>Mirishkor tumani</t>
+        </is>
+      </c>
+      <c r="G225" t="inlineStr">
+        <is>
+          <t>998914655046</t>
+        </is>
+      </c>
+      <c r="H225" t="inlineStr">
+        <is>
+          <t>06-12-2024</t>
+        </is>
+      </c>
+      <c r="I225" t="inlineStr">
+        <is>
+          <t>+998914655046</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Narzullayeva Moxibonu Sharofiddin qizi</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>AC2854766</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>810</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F226" t="inlineStr">
+        <is>
+          <t>Uzun tumani</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>998917962778</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>06-12-2024</t>
+        </is>
+      </c>
+      <c r="I226" t="inlineStr">
+        <is>
+          <t>+998917771900</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Narzullayeva Moxibonu Sharofiddin qizi</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>AC2854766</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>810</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F227" t="inlineStr">
+        <is>
+          <t>Uzun tumani</t>
+        </is>
+      </c>
+      <c r="G227" t="inlineStr">
+        <is>
+          <t>998917962778</t>
+        </is>
+      </c>
+      <c r="H227" t="inlineStr">
+        <is>
+          <t>06-12-2024</t>
+        </is>
+      </c>
+      <c r="I227" t="inlineStr">
+        <is>
+          <t>+998917771900</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Eshpulatova Zilola Tulqinovna</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>AD9498968</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>811</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F228" t="inlineStr">
+        <is>
+          <t>Paxtachi tumani</t>
+        </is>
+      </c>
+      <c r="G228" t="inlineStr">
+        <is>
+          <t>+79962109798</t>
+        </is>
+      </c>
+      <c r="H228" t="inlineStr">
+        <is>
+          <t>07-12-2024</t>
+        </is>
+      </c>
+      <c r="I228" t="inlineStr">
+        <is>
+          <t>+998938377717</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Rahimova Dilafruz Abdujalilovna</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>Amaliy psixologiya 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>AB4431974</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>811</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F229" t="inlineStr">
+        <is>
+          <t>Qarshi tumani</t>
+        </is>
+      </c>
+      <c r="G229" t="inlineStr">
+        <is>
+          <t>998919463549</t>
+        </is>
+      </c>
+      <c r="H229" t="inlineStr">
+        <is>
+          <t>07-12-2024</t>
+        </is>
+      </c>
+      <c r="I229" t="inlineStr">
+        <is>
+          <t>+998886717202</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Raxmonaliyeva Qizlarxon Sarvar qizi</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>AC2065141</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>812</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F230" t="inlineStr">
+        <is>
+          <t>Bagʻdod tumani</t>
+        </is>
+      </c>
+      <c r="G230" t="inlineStr">
+        <is>
+          <t>998908573771</t>
+        </is>
+      </c>
+      <c r="H230" t="inlineStr">
+        <is>
+          <t>07-12-2024</t>
+        </is>
+      </c>
+      <c r="I230" t="inlineStr">
+        <is>
+          <t>+998908573771</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Ishpulatova Zilola Tulqinovna</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>AD9498968</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>813</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>Samarqand viloyati</t>
+        </is>
+      </c>
+      <c r="F231" t="inlineStr">
+        <is>
+          <t>Paxtachi tumani</t>
+        </is>
+      </c>
+      <c r="G231" t="inlineStr">
+        <is>
+          <t>998917962778</t>
+        </is>
+      </c>
+      <c r="H231" t="inlineStr">
+        <is>
+          <t>10-12-2024</t>
+        </is>
+      </c>
+      <c r="I231" t="inlineStr">
+        <is>
+          <t>+998938377717</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Sarsenbaeva Gulmiyra Reyimbay qizi</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>KA0896603</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>814</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F232" t="inlineStr">
+        <is>
+          <t>Chimboy tumani</t>
+        </is>
+      </c>
+      <c r="G232" t="inlineStr">
+        <is>
+          <t>998976501820</t>
+        </is>
+      </c>
+      <c r="H232" t="inlineStr">
+        <is>
+          <t>10-12-2024</t>
+        </is>
+      </c>
+      <c r="I232" t="inlineStr">
+        <is>
+          <t>+998976501820</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Boymatova Volida Siddiq qizi</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>AB7889821</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>815</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="G233" t="inlineStr">
+        <is>
+          <t>998940113792</t>
+        </is>
+      </c>
+      <c r="H233" t="inlineStr">
+        <is>
+          <t>10-12-2024</t>
+        </is>
+      </c>
+      <c r="I233" t="inlineStr">
+        <is>
+          <t>+998940113792</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Norboyeva Hulkar Nuriddinovna</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>AB3950878</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>816</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>Nishon tumani</t>
+        </is>
+      </c>
+      <c r="G234" t="inlineStr">
+        <is>
+          <t>+998991924001</t>
+        </is>
+      </c>
+      <c r="H234" t="inlineStr">
+        <is>
+          <t>10-12-2024</t>
+        </is>
+      </c>
+      <c r="I234" t="inlineStr">
+        <is>
+          <t>+998970620692</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Urmonova Gulnozaxon Tursunaliqizi</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>AA9910161</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>817</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F235" t="inlineStr">
+        <is>
+          <t>Toshloq tumani</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>998901607965</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>11-12-2024</t>
+        </is>
+      </c>
+      <c r="I235" t="inlineStr">
+        <is>
+          <t>+998952342290</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Qo'ldosheva Hafiza Xo'jamaxmatovna</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>AB0558610</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>818</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F236" t="inlineStr">
+        <is>
+          <t>Kasbi tumani</t>
+        </is>
+      </c>
+      <c r="G236" t="inlineStr">
+        <is>
+          <t>998903159740</t>
+        </is>
+      </c>
+      <c r="H236" t="inlineStr">
+        <is>
+          <t>11-12-2024</t>
+        </is>
+      </c>
+      <c r="I236" t="inlineStr">
+        <is>
+          <t>+998503009740</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Rano Ametova Qiriqbay qizi</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>KA0755193</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>819</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>Qoraqalpogʻiston Respublikasi</t>
+        </is>
+      </c>
+      <c r="F237" t="inlineStr">
+        <is>
+          <t>Qoraoʻzak tumani</t>
+        </is>
+      </c>
+      <c r="G237" t="inlineStr">
+        <is>
+          <t>998949011251</t>
+        </is>
+      </c>
+      <c r="H237" t="inlineStr">
+        <is>
+          <t>11-12-2024</t>
+        </is>
+      </c>
+      <c r="I237" t="inlineStr">
+        <is>
+          <t>+998949011251</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Farmonova Nodiraxon Sultanboevna</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>AD7673103</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>820</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F238" t="inlineStr">
+        <is>
+          <t>Paxtaobod tumani</t>
+        </is>
+      </c>
+      <c r="G238" t="inlineStr">
+        <is>
+          <t>998932588722</t>
+        </is>
+      </c>
+      <c r="H238" t="inlineStr">
+        <is>
+          <t>12-12-2024</t>
+        </is>
+      </c>
+      <c r="I238" t="inlineStr">
+        <is>
+          <t>+998935588722</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Jafarova Gulguncha Dostonkulovna</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>AD4523234</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>821</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F239" t="inlineStr">
+        <is>
+          <t>Sariosiyo tumani</t>
+        </is>
+      </c>
+      <c r="G239" t="inlineStr">
+        <is>
+          <t>998991298545</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>12-12-2024</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>+998991298545</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Kurbanova Fazilat Alisherovna</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>AA9895461</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>822</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F240" t="inlineStr">
+        <is>
+          <t>Urganch tumani</t>
+        </is>
+      </c>
+      <c r="G240" t="inlineStr">
+        <is>
+          <t>998999489449</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>13-12-2024</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>+998999489449</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Adilova Gulnoza Xusain qizi</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>AB4655536</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>823</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F241" t="inlineStr">
+        <is>
+          <t>Hazorasp tumani</t>
+        </is>
+      </c>
+      <c r="G241" t="inlineStr">
+        <is>
+          <t>998990188334</t>
+        </is>
+      </c>
+      <c r="H241" t="inlineStr">
+        <is>
+          <t>13-12-2024</t>
+        </is>
+      </c>
+      <c r="I241" t="inlineStr">
+        <is>
+          <t>+998990188334</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Xurshidbekova Feruza Rustamjon qizi</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>AB8629725</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>824</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F242" t="inlineStr">
+        <is>
+          <t>Oltinkoʻl tuman</t>
+        </is>
+      </c>
+      <c r="G242" t="inlineStr">
+        <is>
+          <t>998947244446</t>
+        </is>
+      </c>
+      <c r="H242" t="inlineStr">
+        <is>
+          <t>13-12-2024</t>
+        </is>
+      </c>
+      <c r="I242" t="inlineStr">
+        <is>
+          <t>+998505119296</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Abdiraxmanov Shuxrat Abdinazarovich</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>AB8522464</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>825</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F243" t="inlineStr">
+        <is>
+          <t>Angor tumani</t>
+        </is>
+      </c>
+      <c r="G243" t="inlineStr">
+        <is>
+          <t>+998944610898</t>
+        </is>
+      </c>
+      <c r="H243" t="inlineStr">
+        <is>
+          <t>13-12-2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>QurbonovaShahrizoda Murodaliyevna</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>AC3111040</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>826</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>Yashnaobod tumani</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>998974400150</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>13-12-2024</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>+998974400150</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Mamasoatova Matluba Nurmamat qizi</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>AB3504633</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>827</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F245" t="inlineStr">
+        <is>
+          <t>Gʻuzor tumani</t>
+        </is>
+      </c>
+      <c r="G245" t="inlineStr">
+        <is>
+          <t>+998905884701</t>
+        </is>
+      </c>
+      <c r="H245" t="inlineStr">
+        <is>
+          <t>14-12-2024</t>
+        </is>
+      </c>
+      <c r="I245" t="inlineStr">
+        <is>
+          <t>+998947854245</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Xudjayeva Ra'noxon Qahramonovna</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>AB2244698</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>828</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F246" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G246" t="inlineStr">
+        <is>
+          <t>998881895007</t>
+        </is>
+      </c>
+      <c r="H246" t="inlineStr">
+        <is>
+          <t>16-12-2024</t>
+        </is>
+      </c>
+      <c r="I246" t="inlineStr">
+        <is>
+          <t>+998881895007</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Rahimova Charos Rustamovna</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>AD7563497</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>829</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F247" t="inlineStr">
+        <is>
+          <t>Shovot tumani</t>
+        </is>
+      </c>
+      <c r="G247" t="inlineStr">
+        <is>
+          <t>998999690455</t>
+        </is>
+      </c>
+      <c r="H247" t="inlineStr">
+        <is>
+          <t>16-12-2024</t>
+        </is>
+      </c>
+      <c r="I247" t="inlineStr">
+        <is>
+          <t>+998999690455</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Davronova Gulzoda Mardon qizi</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>AB6474199</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>830</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>Buxoro viloyati</t>
+        </is>
+      </c>
+      <c r="F248" t="inlineStr">
+        <is>
+          <t>Gʻijduvon tumani</t>
+        </is>
+      </c>
+      <c r="G248" t="inlineStr">
+        <is>
+          <t>998972262244</t>
+        </is>
+      </c>
+      <c r="H248" t="inlineStr">
+        <is>
+          <t>16-12-2024</t>
+        </is>
+      </c>
+      <c r="I248" t="inlineStr">
+        <is>
+          <t>+998972262244</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Nazarova Shahriya Murtazoyevna</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>AD8406046</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>831</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F249" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G249" t="inlineStr">
+        <is>
+          <t>998993012335</t>
+        </is>
+      </c>
+      <c r="H249" t="inlineStr">
+        <is>
+          <t>16-12-2024</t>
+        </is>
+      </c>
+      <c r="I249" t="inlineStr">
+        <is>
+          <t>+998993012335</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>Fayzullayeva Muyassar Alimjanovna</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>AA8993904</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>832</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F250" t="inlineStr">
+        <is>
+          <t>Mirobod tumani</t>
+        </is>
+      </c>
+      <c r="G250" t="inlineStr">
+        <is>
+          <t>998973427601</t>
+        </is>
+      </c>
+      <c r="H250" t="inlineStr">
+        <is>
+          <t>16-12-2024</t>
+        </is>
+      </c>
+      <c r="I250" t="inlineStr">
+        <is>
+          <t>+998973427601</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>Bo'riboyev BOBIR Olim o'g'li</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>AD3669106</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>833</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>Jizzax viloyati</t>
+        </is>
+      </c>
+      <c r="F251" t="inlineStr">
+        <is>
+          <t>Baxmal tumani</t>
+        </is>
+      </c>
+      <c r="G251" t="inlineStr">
+        <is>
+          <t>+998946664457</t>
+        </is>
+      </c>
+      <c r="H251" t="inlineStr">
+        <is>
+          <t>18-12-2024</t>
+        </is>
+      </c>
+      <c r="I251" t="inlineStr">
+        <is>
+          <t>+998946664457</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Beknazarova Guljaxon Abdumalik qizi</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>AD7323572</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>834</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>Sirdaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>Mirzaobod tumani</t>
+        </is>
+      </c>
+      <c r="G252" t="inlineStr">
+        <is>
+          <t>998906810212</t>
+        </is>
+      </c>
+      <c r="H252" t="inlineStr">
+        <is>
+          <t>18-12-2024</t>
+        </is>
+      </c>
+      <c r="I252" t="inlineStr">
+        <is>
+          <t>+998906810212</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>Iskandarova Mashhura Shuhrat qizi</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>AD7167198</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>835</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>Xonqa tumani</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>998996256305</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>18-12-2024</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>+998996256305</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Turayeva Gulsanam Xudoynazarovna</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>AB5278176</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>836</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F254" t="inlineStr">
+        <is>
+          <t>Chilonzor tumani</t>
+        </is>
+      </c>
+      <c r="G254" t="inlineStr">
+        <is>
+          <t>998933912282</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>18-12-2024</t>
+        </is>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>+998983142282</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Hakimova Muxlisa Istam qizi</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>AD7312729</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>837</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F255" t="inlineStr">
+        <is>
+          <t>Navoiy shahri</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>998913379383</t>
+        </is>
+      </c>
+      <c r="H255" t="inlineStr">
+        <is>
+          <t>18-12-2024</t>
+        </is>
+      </c>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>+998913379383</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Kirgizbaeva Nodira Alimdjan qizi</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>AC2807349</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>838</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F256" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>998998422061</t>
+        </is>
+      </c>
+      <c r="H256" t="inlineStr">
+        <is>
+          <t>18-12-2024</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
+        <is>
+          <t>+998998422061</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>Akatova Lobar Bahodir qizi</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>AD5687176</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>839</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F257" t="inlineStr">
+        <is>
+          <t>Karmana tumani</t>
+        </is>
+      </c>
+      <c r="G257" t="inlineStr">
+        <is>
+          <t>998997442526</t>
+        </is>
+      </c>
+      <c r="H257" t="inlineStr">
+        <is>
+          <t>19-12-2024</t>
+        </is>
+      </c>
+      <c r="I257" t="inlineStr">
+        <is>
+          <t>+998997442526</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>Masharipova Zilola Xamro Qizi</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>AC0347449</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>840</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F258" t="inlineStr">
+        <is>
+          <t>Shovot tumani</t>
+        </is>
+      </c>
+      <c r="G258" t="inlineStr">
+        <is>
+          <t>998951885515</t>
+        </is>
+      </c>
+      <c r="H258" t="inlineStr">
+        <is>
+          <t>20-12-2024</t>
+        </is>
+      </c>
+      <c r="I258" t="inlineStr">
+        <is>
+          <t>+998914258505</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Roziboyeva Gulhayo Mirzakarimovna</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>AB0903249</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>841</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F259" t="inlineStr">
+        <is>
+          <t>Qoʻrgʻontepa tumani</t>
+        </is>
+      </c>
+      <c r="G259" t="inlineStr">
+        <is>
+          <t>998932001313</t>
+        </is>
+      </c>
+      <c r="H259" t="inlineStr">
+        <is>
+          <t>20-12-2024</t>
+        </is>
+      </c>
+      <c r="I259" t="inlineStr">
+        <is>
+          <t>+998932001313</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>Shixnazarova Nargiza Zinaddin qizi</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>AB7915547</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>842</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F260" t="inlineStr">
+        <is>
+          <t>Xonqa tumani</t>
+        </is>
+      </c>
+      <c r="G260" t="inlineStr">
+        <is>
+          <t>998940944711</t>
+        </is>
+      </c>
+      <c r="H260" t="inlineStr">
+        <is>
+          <t>21-12-2024</t>
+        </is>
+      </c>
+      <c r="I260" t="inlineStr">
+        <is>
+          <t>+998940944711</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Tojiboyeva Ra'noxon Tursunboyevna</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>AB0921764</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>843</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F261" t="inlineStr">
+        <is>
+          <t>Rishton tumani</t>
+        </is>
+      </c>
+      <c r="G261" t="inlineStr">
+        <is>
+          <t>998904091350</t>
+        </is>
+      </c>
+      <c r="H261" t="inlineStr">
+        <is>
+          <t>21-12-2024</t>
+        </is>
+      </c>
+      <c r="I261" t="inlineStr">
+        <is>
+          <t>+998904091350</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Sharaximova Saida Ulugbekovna</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>AD3462669</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>844</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>Toshkent viloyati</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>Zangiota tumani</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>998997991050</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>23-12-2024</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>+998997991050</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Ahmedjonova Dinora Ulugbek qizi</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>AD6661150</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>845</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>Xorazm viloyati</t>
+        </is>
+      </c>
+      <c r="F263" t="inlineStr">
+        <is>
+          <t>Tuproqqalʼa tumani</t>
+        </is>
+      </c>
+      <c r="G263" t="inlineStr">
+        <is>
+          <t>998996240929</t>
+        </is>
+      </c>
+      <c r="H263" t="inlineStr">
+        <is>
+          <t>23-12-2024</t>
+        </is>
+      </c>
+      <c r="I263" t="inlineStr">
+        <is>
+          <t>+998996240929</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Rajabova Yulduz Salomovna</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>AB0844299</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>846</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F264" t="inlineStr">
+        <is>
+          <t>Uzun tumani</t>
+        </is>
+      </c>
+      <c r="G264" t="inlineStr">
+        <is>
+          <t>998994212677</t>
+        </is>
+      </c>
+      <c r="H264" t="inlineStr">
+        <is>
+          <t>24-12-2024</t>
+        </is>
+      </c>
+      <c r="I264" t="inlineStr">
+        <is>
+          <t>+998994212677</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Xujamkulova Zulayxo Xolovna</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>AA9964008</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>847</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>Uzun tumani</t>
+        </is>
+      </c>
+      <c r="G265" t="inlineStr">
+        <is>
+          <t>998902675161</t>
+        </is>
+      </c>
+      <c r="H265" t="inlineStr">
+        <is>
+          <t>24-12-2024</t>
+        </is>
+      </c>
+      <c r="I265" t="inlineStr">
+        <is>
+          <t>+998902675161</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Isaqova Fotima Nomonjonovna</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>AB9045975</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>848</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>Fargʻona tumani</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>+998337830001</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>25-12-2024</t>
+        </is>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>+998936998600</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Dexqonova Dilovar Bakirjon qizi</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>AB8131499</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>849</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F267" t="inlineStr">
+        <is>
+          <t>Buvayda tumani</t>
+        </is>
+      </c>
+      <c r="G267" t="inlineStr">
+        <is>
+          <t>998975558949</t>
+        </is>
+      </c>
+      <c r="H267" t="inlineStr">
+        <is>
+          <t>25-12-2024</t>
+        </is>
+      </c>
+      <c r="I267" t="inlineStr">
+        <is>
+          <t>+998975558949</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Ergasheva Omadoy Maxmudjon qizi</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>AB5700411</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>850</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F268" t="inlineStr">
+        <is>
+          <t>Izboskan tuman</t>
+        </is>
+      </c>
+      <c r="G268" t="inlineStr">
+        <is>
+          <t>998994315229</t>
+        </is>
+      </c>
+      <c r="H268" t="inlineStr">
+        <is>
+          <t>25-12-2024</t>
+        </is>
+      </c>
+      <c r="I268" t="inlineStr">
+        <is>
+          <t>+998994315229</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Sadirova Durdonaxon Xotamxoja qizi</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>AB5666734</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>851</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F269" t="inlineStr">
+        <is>
+          <t>Sergeli tumani</t>
+        </is>
+      </c>
+      <c r="G269" t="inlineStr">
+        <is>
+          <t>998951104303</t>
+        </is>
+      </c>
+      <c r="H269" t="inlineStr">
+        <is>
+          <t>25-12-2024</t>
+        </is>
+      </c>
+      <c r="I269" t="inlineStr">
+        <is>
+          <t>+998951104303</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>Farmonqulova Sayyora Raximovna</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>AD5388355</t>
+        </is>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>852</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F270" t="inlineStr">
+        <is>
+          <t>Yakkasaroy tumani</t>
+        </is>
+      </c>
+      <c r="G270" t="inlineStr">
+        <is>
+          <t>998903362499</t>
+        </is>
+      </c>
+      <c r="H270" t="inlineStr">
+        <is>
+          <t>27-12-2024</t>
+        </is>
+      </c>
+      <c r="I270" t="inlineStr">
+        <is>
+          <t>+998983061940</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>TILLYAYEVA MUATTARXON MUXIDDIN QIZI</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>AB0563656</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>853</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>Jalaquduq tuman</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>998942520806</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>27-12-2024</t>
+        </is>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>+998942520806</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>TILLYAYEVA MUATTARXON MUXIDDIN QIZI</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Defektologiya (logopediya) 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>AB0563956</t>
+        </is>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>854</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr">
+        <is>
+          <t>Andijon viloyati</t>
+        </is>
+      </c>
+      <c r="F272" t="inlineStr">
+        <is>
+          <t>Jalaquduq tuman</t>
+        </is>
+      </c>
+      <c r="G272" t="inlineStr">
+        <is>
+          <t>998905496444</t>
+        </is>
+      </c>
+      <c r="H272" t="inlineStr">
+        <is>
+          <t>27-12-2024</t>
+        </is>
+      </c>
+      <c r="I272" t="inlineStr">
+        <is>
+          <t>+998942520806</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>TOSHKUZIYEVA KHUSNIDAKHON GAYRATJON QIZI</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>AA9652025</t>
+        </is>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>855</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr">
+        <is>
+          <t>Fargona viloyati</t>
+        </is>
+      </c>
+      <c r="F273" t="inlineStr">
+        <is>
+          <t>Bagʻdod tumani</t>
+        </is>
+      </c>
+      <c r="G273" t="inlineStr">
+        <is>
+          <t>998903627656</t>
+        </is>
+      </c>
+      <c r="H273" t="inlineStr">
+        <is>
+          <t>27-12-2024</t>
+        </is>
+      </c>
+      <c r="I273" t="inlineStr">
+        <is>
+          <t>+998903627656</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>Dusanov Chori Shermatovich</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>AB0618829</t>
+        </is>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>855</t>
+        </is>
+      </c>
+      <c r="E274" t="inlineStr">
+        <is>
+          <t>Surxondaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F274" t="inlineStr">
+        <is>
+          <t>Boysun tumani</t>
+        </is>
+      </c>
+      <c r="G274" t="inlineStr">
+        <is>
+          <t>998770468177</t>
+        </is>
+      </c>
+      <c r="H274" t="inlineStr">
+        <is>
+          <t>03-01-2025</t>
+        </is>
+      </c>
+      <c r="I274" t="inlineStr">
+        <is>
+          <t>+998919818177</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
13:55 time 03.03.2025 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Asosiy\Teloegram_bot_P\MTT_kontrakt\file_service\file_database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm\MTT_kontrakt\file_service\file_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33945640-A1FB-442A-A182-DCAEA99375D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0D552C-A3AB-440D-976F-AAC3F90EA864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,13 +46,13 @@
     <t>Sana</t>
   </si>
   <si>
-    <t>Amirov AKrom</t>
-  </si>
-  <si>
-    <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
-  </si>
-  <si>
-    <t>AA7778899</t>
+    <t>Amirov Akrom</t>
+  </si>
+  <si>
+    <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+  </si>
+  <si>
+    <t>AB9890099</t>
   </si>
   <si>
     <t>056</t>
@@ -447,7 +447,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
15:32 time 17.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -1,95 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pycharm\MTT_kontrakt\file_service\file_database\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0D552C-A3AB-440D-976F-AAC3F90EA864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>F.I.SH</t>
-  </si>
-  <si>
-    <t>Ta'lim yo'nalishi</t>
-  </si>
-  <si>
-    <t>Passport</t>
-  </si>
-  <si>
-    <t>Shartnoma raqam</t>
-  </si>
-  <si>
-    <t>Viloyat</t>
-  </si>
-  <si>
-    <t>Tuman</t>
-  </si>
-  <si>
-    <t>Telefon raqam</t>
-  </si>
-  <si>
-    <t>Sana</t>
-  </si>
-  <si>
-    <t>Amirov Akrom</t>
-  </si>
-  <si>
-    <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
-  </si>
-  <si>
-    <t>AB9890099</t>
-  </si>
-  <si>
-    <t>056</t>
-  </si>
-  <si>
-    <t>Navoiy viloyati</t>
-  </si>
-  <si>
-    <t>Xatirchi tumani</t>
-  </si>
-  <si>
-    <t>+12676860109</t>
-  </si>
-  <si>
-    <t>03-03-2025</t>
-  </si>
-  <si>
-    <t>+998945289910</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -123,27 +62,86 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -443,82 +441,263 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="42.85546875" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" customWidth="1"/>
+    <col width="42.85546875" customWidth="1" min="1" max="1"/>
+    <col width="49.85546875" customWidth="1" min="2" max="2"/>
+    <col width="16.85546875" customWidth="1" min="3" max="3"/>
+    <col width="10.42578125" customWidth="1" min="4" max="4"/>
+    <col width="45.85546875" customWidth="1" min="5" max="5"/>
+    <col width="41" customWidth="1" min="6" max="6"/>
+    <col width="18.28515625" customWidth="1" min="7" max="7"/>
+    <col width="18.140625" customWidth="1" min="8" max="8"/>
+    <col width="18.28515625" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
+    <row r="1" ht="38.25" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>F.I.SH</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Ta'lim yo'nalishi</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Passport</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Shartnoma raqam</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Viloyat</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tuman</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Telefon raqam</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Sana</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Telefon raqam</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Amirov Akrom</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AB9890099</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>056</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Navoiy viloyati</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Xatirchi tumani</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>+12676860109</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>03-03-2025</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>+998945289910</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Tursunxojayev Xasanxoja Marufxon ogli</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AB0865260</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>057</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Namangan viloyati</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Yangiqoʻrgʻon tumani</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>+998935925257</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>03-03-2025</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>+998935925257</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Matkarimova Manzuraxon Raxmonaliyevna</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AD4917676</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>058</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sirdaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Sirdaryo tumani</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>998999286588</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>11-03-2025</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>+998999286588</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Axtamov Abduraxim  Axtamovich</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 864 soatlik</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>AD1234567</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>059</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Toshkent shahri</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Yunusobod tumani</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>+998942239090</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>02-04-2025</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>+998919404001</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
12:21 time 21.04.2025 date
</commit_message>
<xml_diff>
--- a/file_service/file_database/qabul.xlsx
+++ b/file_service/file_database/qabul.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -700,6 +700,53 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Giyosov Azizbek Ilhomovich</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Maktabgacha ta’lim tashkiloti tarbiyachisi 576 soatlik</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>AD0993829</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>060</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Qashqadaryo viloyati</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Koson tumani</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>998972903393</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>21-04-2025</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>+998972903393</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>